<commit_message>
Initial support for cite-seq data
</commit_message>
<xml_diff>
--- a/tcrdb/resources/web/tcrdb/exampleData/ImportReadsetTemplate.xlsx
+++ b/tcrdb/resources/web/tcrdb/exampleData/ImportReadsetTemplate.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>5' GEX Index</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>Workbook</t>
+  </si>
+  <si>
+    <t>CITE-seq Library Index</t>
+  </si>
+  <si>
+    <t>CITE-seq Library Conc</t>
   </si>
 </sst>
 </file>
@@ -392,11 +398,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -408,8 +412,8 @@
     <col min="6" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:10" s="3" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="5" t="s">
@@ -433,26 +437,32 @@
       <c r="H1" s="5" t="s">
         <v>1</v>
       </c>
+      <c r="I1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>

</xml_diff>